<commit_message>
maxico input file changed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BA7549-9D1C-42EE-9918-4D85E5D760DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C158B5-7AD1-486F-931B-10B32A1429F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="345" windowWidth="16140" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -283,25 +283,25 @@
     <t>rhernandez@tecnoyar.com.mx</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envio Semana 06/MÉXICO/Base de Datos/Consolidado</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/Base de Datos/Exportadas</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/Mi Cine</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/Tradicional</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/Atmosfera</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/06 Envío Semana 06/MÉXICO/VIP</t>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/MÉXICO/Base de Datos/Consolidado</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Tradicional</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Mi Cine</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Atmosfera</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -816,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -842,7 +842,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -868,7 +868,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
         <v>71</v>
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75">
@@ -895,7 +895,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -907,7 +907,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -919,7 +919,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75">
@@ -931,7 +931,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -951,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -967,7 +967,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -983,7 +983,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1021,7 +1021,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1115,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1307,7 +1307,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="27">
-        <v>44592</v>
+        <v>44585</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>64</v>
@@ -1318,7 +1318,7 @@
         <v>62</v>
       </c>
       <c r="B25" s="27">
-        <v>44598</v>
+        <v>44591</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
process updated for testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C158B5-7AD1-486F-931B-10B32A1429F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8FCAD5-56C2-41D9-B14B-25482DA2DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4755" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -816,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
process updated for final maxico
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\cinepolisMaxico\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8FCAD5-56C2-41D9-B14B-25482DA2DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD23DC1-CA0D-49DB-910D-4258E6B831C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -281,25 +281,25 @@
     <t>rhernandez@tecnoyar.com.mx</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/MÉXICO/Base de Datos/Consolidado</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Tradicional</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Mi Cine</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Atmosfera</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/05 Envío Semana 05/MÉXICO/Base de Datos/Exportadas</t>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envio Semana 07/MÉXICO/Base de Datos/Consolidado</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Tradicional</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Mi Cine</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Atmosfera</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1305,7 +1305,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="27">
-        <v>44585</v>
+        <v>44599</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>64</v>
@@ -1316,7 +1316,7 @@
         <v>62</v>
       </c>
       <c r="B25" s="27">
-        <v>44591</v>
+        <v>44605</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
process updated for correct name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD23DC1-CA0D-49DB-910D-4258E6B831C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8812BD3F-BBA5-4B19-9C00-EFC29996FE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>CorrectSheetName</t>
+  </si>
+  <si>
+    <t>Keywords in filename</t>
   </si>
 </sst>
 </file>
@@ -812,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -824,7 +833,7 @@
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,8 +843,11 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -846,22 +858,22 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="21"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2"/>
       <c r="B5" s="21"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -872,11 +884,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="2"/>
       <c r="B7" s="21"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -884,11 +896,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="2"/>
       <c r="B9" s="21"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:4" ht="15.75">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -896,11 +908,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="22"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -908,11 +920,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
+    <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -920,11 +932,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="2"/>
       <c r="B15" s="21"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:4" ht="15.75">
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
@@ -1099,6 +1111,18 @@
       <c r="B45" s="21" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75">
+      <c r="A47" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="21"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.75">
+      <c r="A48" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1113,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
process tested and updated for blacklist file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\cinepolisMaxico\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8812BD3F-BBA5-4B19-9C00-EFC29996FE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E30376B-DEDF-40A2-92FB-85A098E4DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>Keywords in filename</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/1 Directorio/Correcciones</t>
+  </si>
+  <si>
+    <t>Hoja</t>
+  </si>
+  <si>
+    <t>CORRECCIONES</t>
   </si>
 </sst>
 </file>
@@ -823,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,7 +1035,7 @@
     <row r="31" spans="1:2">
       <c r="A31" s="2"/>
     </row>
-    <row r="33" spans="1:2" ht="15.75">
+    <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>
@@ -1042,10 +1051,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:2" ht="15.75">
+    <row r="36" spans="1:4" ht="15.75">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>65</v>
       </c>
@@ -1061,10 +1070,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75">
+    <row r="44" spans="1:4" ht="15.75">
       <c r="A44" s="21" t="s">
         <v>26</v>
       </c>
@@ -1104,7 +1113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75">
+    <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="21" t="s">
         <v>27</v>
       </c>
@@ -1112,17 +1121,24 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75">
+    <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="21"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.75">
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="21"/>
+      <c r="B48" s="21" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
maxico special character done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E30376B-DEDF-40A2-92FB-85A098E4DB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7A8001-E362-4D34-ADF6-2D78F5AB9D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -281,27 +281,6 @@
     <t>rhernandez@tecnoyar.com.mx</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envio Semana 07/MÉXICO/Base de Datos/Consolidado</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Tradicional</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Mi Cine</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Atmosfera</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/MÉXICO/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>CorrectnameFilePath</t>
   </si>
   <si>
@@ -318,13 +297,34 @@
   </si>
   <si>
     <t>CORRECCIONES</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envio Semana 09/MÉXICO/Base de Datos/Consolidado</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Tradicional</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Mi Cine</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Atmosfera</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -446,6 +446,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -467,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -516,6 +523,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53:C54"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
@@ -861,7 +869,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>70</v>
@@ -871,6 +879,7 @@
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
@@ -887,7 +896,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
         <v>71</v>
@@ -902,7 +911,7 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75">
@@ -914,7 +923,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -926,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -938,7 +947,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
@@ -950,7 +959,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -962,7 +971,7 @@
         <v>61</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75">
@@ -970,7 +979,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -986,7 +995,7 @@
         <v>44</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1002,7 +1011,7 @@
         <v>45</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1021,7 +1030,7 @@
         <v>46</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1040,7 +1049,7 @@
         <v>50</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1123,21 +1132,21 @@
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="21" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1153,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z981"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1345,7 +1354,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="27">
-        <v>44599</v>
+        <v>44613</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>64</v>
@@ -1356,7 +1365,7 @@
         <v>62</v>
       </c>
       <c r="B25" s="27">
-        <v>44605</v>
+        <v>44619</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
name issue is fixed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\cinepolisMaxico\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7A8001-E362-4D34-ADF6-2D78F5AB9D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B65397-8C8B-4932-8806-B2C9E9958DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,25 +299,25 @@
     <t>CORRECCIONES</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envio Semana 09/MÉXICO/Base de Datos/Consolidado</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Tradicional</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Mi Cine</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Atmosfera</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/MÉXICO/Base de Datos/Exportadas</t>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envio Semana 10/MÉXICO/Base de Datos/Consolidado</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/Tradicional</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/Mi Cine</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/Atmosfera</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/10 Envío Semana 10/MÉXICO/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:Z981"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1354,7 +1354,7 @@
         <v>63</v>
       </c>
       <c r="B24" s="27">
-        <v>44613</v>
+        <v>44621</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>64</v>
@@ -1365,7 +1365,7 @@
         <v>62</v>
       </c>
       <c r="B25" s="27">
-        <v>44619</v>
+        <v>44626</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>64</v>

</xml_diff>